<commit_message>
LITE-28859 Eased PPR validation (made it open)
* Now we check only if required columns exist
* Non-required columns are allowed but affect nothing
</commit_message>
<xml_diff>
--- a/tests/fixtures/test_PPR_file_invalid.xlsx
+++ b/tests/fixtures/test_PPR_file_invalid.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igrebenshikov00/GIT/connect-extension-xvs/tests/fixtures/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/max/code/connect-extension-xvs/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B6AEF9-2D80-8A44-A8B1-232FC214AED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D35A3B9-914C-6640-B34A-0408EA482137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="163">
   <si>
     <t>Name_EN</t>
   </si>
@@ -543,7 +543,7 @@
     <t>BillingAlignmentResellerRedefineAllowed</t>
   </si>
   <si>
-    <t>Smth else</t>
+    <t>MPÑ</t>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -965,7 +965,7 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -987,7 +987,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>162</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -995,9 +995,7 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>162</v>
-      </c>
+      <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>

</xml_diff>